<commit_message>
updated Zn-NiO ellipsometry data
</commit_message>
<xml_diff>
--- a/Ellipsometry/NiO_011620.xlsx
+++ b/Ellipsometry/NiO_011620.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/KINGSTON/Michigan 2018/Data/Ellipsometry/otrejo/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A435C312-9CAD-594D-9CE6-CBAB0DF13C19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="18200" windowHeight="11560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="465" windowWidth="18195" windowHeight="11565" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NiO" sheetId="1" r:id="rId1"/>
+    <sheet name="Zn-NiO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Position (cm)</t>
   </si>
@@ -115,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,26 +235,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,23 +270,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,16 +445,639 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1.863</v>
+      </c>
+      <c r="C2">
+        <v>85.16</v>
+      </c>
+      <c r="D2">
+        <v>1.5424</v>
+      </c>
+      <c r="E2">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="F2">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="G2">
+        <v>98.16</v>
+      </c>
+      <c r="H2">
+        <v>1.784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1.619</v>
+      </c>
+      <c r="C3">
+        <v>83.52</v>
+      </c>
+      <c r="D3">
+        <v>1.5248999999999999</v>
+      </c>
+      <c r="E3">
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="G3">
+        <v>96.52</v>
+      </c>
+      <c r="H3">
+        <v>1.7673000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2.1240000000000001</v>
+      </c>
+      <c r="C4">
+        <v>87.47</v>
+      </c>
+      <c r="D4">
+        <v>1.5928</v>
+      </c>
+      <c r="E4">
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="F4">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="G4">
+        <v>100.47</v>
+      </c>
+      <c r="H4">
+        <v>1.8005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.04</v>
+      </c>
+      <c r="D5">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="E5">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="F5">
+        <v>1E-3</v>
+      </c>
+      <c r="G5">
+        <v>1.04</v>
+      </c>
+      <c r="H5">
+        <v>1.15E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>13.555</v>
+      </c>
+      <c r="C6">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D6">
+        <v>2.2040000000000002</v>
+      </c>
+      <c r="E6">
+        <v>21.282699999999998</v>
+      </c>
+      <c r="F6">
+        <v>19.552399999999999</v>
+      </c>
+      <c r="G6">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="H6">
+        <v>0.92969999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>2.0110000000000001</v>
+      </c>
+      <c r="C7">
+        <v>85.11</v>
+      </c>
+      <c r="D7">
+        <v>1.5259</v>
+      </c>
+      <c r="E7">
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="F7">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="G7">
+        <v>98.11</v>
+      </c>
+      <c r="H7">
+        <v>1.7904</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1.96</v>
+      </c>
+      <c r="C8">
+        <v>84.98</v>
+      </c>
+      <c r="D8">
+        <v>1.5435000000000001</v>
+      </c>
+      <c r="E8">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="F8">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G8">
+        <v>97.98</v>
+      </c>
+      <c r="H8">
+        <v>1.7984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>2.0840000000000001</v>
+      </c>
+      <c r="C9">
+        <v>85.58</v>
+      </c>
+      <c r="D9">
+        <v>1.5474000000000001</v>
+      </c>
+      <c r="E9">
+        <v>8.48E-2</v>
+      </c>
+      <c r="F9">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G9">
+        <v>98.58</v>
+      </c>
+      <c r="H9">
+        <v>1.8004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>1.895</v>
+      </c>
+      <c r="C10">
+        <v>86.03</v>
+      </c>
+      <c r="D10">
+        <v>1.5383</v>
+      </c>
+      <c r="E10">
+        <v>8.5199999999999998E-2</v>
+      </c>
+      <c r="F10">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G10">
+        <v>99.03</v>
+      </c>
+      <c r="H10">
+        <v>1.7949999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1.889</v>
+      </c>
+      <c r="C11">
+        <v>85.9</v>
+      </c>
+      <c r="D11">
+        <v>1.5256000000000001</v>
+      </c>
+      <c r="E11">
+        <v>8.1799999999999998E-2</v>
+      </c>
+      <c r="F11">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G11">
+        <v>98.9</v>
+      </c>
+      <c r="H11">
+        <v>1.7798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>1.7430000000000001</v>
+      </c>
+      <c r="C12">
+        <v>85.21</v>
+      </c>
+      <c r="D12">
+        <v>1.5248999999999999</v>
+      </c>
+      <c r="E12">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F12">
+        <v>8.6E-3</v>
+      </c>
+      <c r="G12">
+        <v>98.21</v>
+      </c>
+      <c r="H12">
+        <v>1.7730999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>1.762</v>
+      </c>
+      <c r="C13">
+        <v>84.41</v>
+      </c>
+      <c r="D13">
+        <v>1.5286</v>
+      </c>
+      <c r="E13">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="G13">
+        <v>97.41</v>
+      </c>
+      <c r="H13">
+        <v>1.7694000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>2.1240000000000001</v>
+      </c>
+      <c r="C14">
+        <v>84.29</v>
+      </c>
+      <c r="D14">
+        <v>1.532</v>
+      </c>
+      <c r="E14">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="F14">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G14">
+        <v>97.29</v>
+      </c>
+      <c r="H14">
+        <v>1.7766999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>1.89</v>
+      </c>
+      <c r="C15">
+        <v>84.81</v>
+      </c>
+      <c r="D15">
+        <v>1.5357000000000001</v>
+      </c>
+      <c r="E15">
+        <v>7.9299999999999995E-2</v>
+      </c>
+      <c r="F15">
+        <v>7.6E-3</v>
+      </c>
+      <c r="G15">
+        <v>97.81</v>
+      </c>
+      <c r="H15">
+        <v>1.7813000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>1.7290000000000001</v>
+      </c>
+      <c r="C16">
+        <v>84.56</v>
+      </c>
+      <c r="D16">
+        <v>1.5928</v>
+      </c>
+      <c r="E16">
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="F16">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="G16">
+        <v>97.56</v>
+      </c>
+      <c r="H16">
+        <v>1.7866</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>1.869</v>
+      </c>
+      <c r="C17">
+        <v>84.39</v>
+      </c>
+      <c r="D17">
+        <v>1.5633999999999999</v>
+      </c>
+      <c r="E17">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="F17">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="G17">
+        <v>97.39</v>
+      </c>
+      <c r="H17">
+        <v>1.7965</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>1.619</v>
+      </c>
+      <c r="C18">
+        <v>83.83</v>
+      </c>
+      <c r="D18">
+        <v>1.5407</v>
+      </c>
+      <c r="E18">
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="F18">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="G18">
+        <v>96.83</v>
+      </c>
+      <c r="H18">
+        <v>1.7673000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="C19">
+        <v>83.52</v>
+      </c>
+      <c r="D19">
+        <v>1.5436000000000001</v>
+      </c>
+      <c r="E19">
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="F19">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="G19">
+        <v>96.52</v>
+      </c>
+      <c r="H19">
+        <v>1.7713000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="C20">
+        <v>84.88</v>
+      </c>
+      <c r="D20">
+        <v>1.5344</v>
+      </c>
+      <c r="E20">
+        <v>7.5399999999999995E-2</v>
+      </c>
+      <c r="F20">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G20">
+        <v>97.88</v>
+      </c>
+      <c r="H20">
+        <v>1.7757000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>1.718</v>
+      </c>
+      <c r="C21">
+        <v>86.98</v>
+      </c>
+      <c r="D21">
+        <v>1.5325</v>
+      </c>
+      <c r="E21">
+        <v>7.6399999999999996E-2</v>
+      </c>
+      <c r="F21">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="G21">
+        <v>99.98</v>
+      </c>
+      <c r="H21">
+        <v>1.7750999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="C22">
+        <v>87.47</v>
+      </c>
+      <c r="D22">
+        <v>1.5396000000000001</v>
+      </c>
+      <c r="E22">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="F22">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="G22">
+        <v>100.47</v>
+      </c>
+      <c r="H22">
+        <v>1.7907</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>1.9179999999999999</v>
+      </c>
+      <c r="C23">
+        <v>85.77</v>
+      </c>
+      <c r="D23">
+        <v>1.5713999999999999</v>
+      </c>
+      <c r="E23">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="F23">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="G23">
+        <v>98.77</v>
+      </c>
+      <c r="H23">
+        <v>1.8005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H23"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,576 +1103,576 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1.863</v>
+        <v>2.62</v>
       </c>
       <c r="C2">
-        <v>85.16</v>
+        <v>164.88</v>
       </c>
       <c r="D2">
-        <v>1.5424</v>
+        <v>2.1139000000000001</v>
       </c>
       <c r="E2">
-        <v>7.7100000000000002E-2</v>
+        <v>-1.0500000000000001E-2</v>
       </c>
       <c r="F2">
-        <v>7.9000000000000008E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="G2">
-        <v>98.16</v>
+        <v>179.88</v>
       </c>
       <c r="H2">
-        <v>1.784</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1581999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>1.619</v>
+        <v>2.214</v>
       </c>
       <c r="C3">
-        <v>83.52</v>
+        <v>161.94999999999999</v>
       </c>
       <c r="D3">
-        <v>1.5248999999999999</v>
+        <v>2.0708000000000002</v>
       </c>
       <c r="E3">
-        <v>5.5500000000000001E-2</v>
+        <v>-2.6499999999999999E-2</v>
       </c>
       <c r="F3">
-        <v>6.4000000000000003E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="G3">
-        <v>96.52</v>
+        <v>176.95</v>
       </c>
       <c r="H3">
-        <v>1.7673000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1474000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4">
-        <v>2.1240000000000001</v>
+        <v>2.84</v>
       </c>
       <c r="C4">
-        <v>87.47</v>
+        <v>167.55</v>
       </c>
       <c r="D4">
-        <v>1.5928</v>
+        <v>2.1423000000000001</v>
       </c>
       <c r="E4">
-        <v>8.8300000000000003E-2</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="F4">
-        <v>9.4999999999999998E-3</v>
+        <v>1.34E-2</v>
       </c>
       <c r="G4">
-        <v>100.47</v>
+        <v>182.55</v>
       </c>
       <c r="H4">
-        <v>1.8005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1692</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.13900000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="C5">
-        <v>1.04</v>
+        <v>1.47</v>
       </c>
       <c r="D5">
-        <v>1.8100000000000002E-2</v>
+        <v>2.2800000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>8.2000000000000007E-3</v>
+        <v>1.11E-2</v>
       </c>
       <c r="F5">
-        <v>1E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G5">
-        <v>1.04</v>
+        <v>1.47</v>
       </c>
       <c r="H5">
-        <v>1.15E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>13.555</v>
+        <v>11.957000000000001</v>
       </c>
       <c r="C6">
-        <v>2.3199999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="D6">
-        <v>2.2040000000000002</v>
+        <v>1.6912</v>
       </c>
       <c r="E6">
-        <v>21.282699999999998</v>
+        <v>-177.50319999999999</v>
       </c>
       <c r="F6">
-        <v>19.552399999999999</v>
+        <v>23.119299999999999</v>
       </c>
       <c r="G6">
-        <v>2.0099999999999998</v>
+        <v>1.56</v>
       </c>
       <c r="H6">
-        <v>0.92969999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.50470000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>2.0110000000000001</v>
+        <v>2.5880000000000001</v>
       </c>
       <c r="C7">
-        <v>85.11</v>
+        <v>166.16</v>
       </c>
       <c r="D7">
-        <v>1.5259</v>
+        <v>2.1280999999999999</v>
       </c>
       <c r="E7">
-        <v>8.8300000000000003E-2</v>
+        <v>-1.2200000000000001E-2</v>
       </c>
       <c r="F7">
-        <v>7.1000000000000004E-3</v>
+        <v>1.15E-2</v>
       </c>
       <c r="G7">
-        <v>98.11</v>
+        <v>181.16</v>
       </c>
       <c r="H7">
-        <v>1.7904</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1692</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>1.96</v>
+        <v>2.41</v>
       </c>
       <c r="C8">
-        <v>84.98</v>
+        <v>166.46</v>
       </c>
       <c r="D8">
-        <v>1.5435000000000001</v>
+        <v>2.1181000000000001</v>
       </c>
       <c r="E8">
-        <v>8.5599999999999996E-2</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="F8">
-        <v>6.6E-3</v>
+        <v>1.09E-2</v>
       </c>
       <c r="G8">
-        <v>97.98</v>
+        <v>181.46</v>
       </c>
       <c r="H8">
-        <v>1.7984</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1640000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>2.0840000000000001</v>
+        <v>2.673</v>
       </c>
       <c r="C9">
-        <v>85.58</v>
+        <v>165.8</v>
       </c>
       <c r="D9">
-        <v>1.5474000000000001</v>
+        <v>2.1191</v>
       </c>
       <c r="E9">
-        <v>8.48E-2</v>
+        <v>-1.1299999999999999E-2</v>
       </c>
       <c r="F9">
-        <v>6.6E-3</v>
+        <v>1.14E-2</v>
       </c>
       <c r="G9">
-        <v>98.58</v>
+        <v>180.8</v>
       </c>
       <c r="H9">
-        <v>1.8004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1621000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>1.895</v>
+        <v>2.7290000000000001</v>
       </c>
       <c r="C10">
-        <v>86.03</v>
+        <v>165.07</v>
       </c>
       <c r="D10">
-        <v>1.5383</v>
+        <v>2.1231</v>
       </c>
       <c r="E10">
-        <v>8.5199999999999998E-2</v>
+        <v>-1.43E-2</v>
       </c>
       <c r="F10">
-        <v>7.0000000000000001E-3</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="G10">
-        <v>99.03</v>
+        <v>180.07</v>
       </c>
       <c r="H10">
-        <v>1.7949999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1614</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11">
-        <v>1.889</v>
+        <v>2.677</v>
       </c>
       <c r="C11">
-        <v>85.9</v>
+        <v>164.89</v>
       </c>
       <c r="D11">
-        <v>1.5256000000000001</v>
+        <v>2.1219000000000001</v>
       </c>
       <c r="E11">
-        <v>8.1799999999999998E-2</v>
+        <v>-1.3899999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>8.0000000000000002E-3</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="G11">
-        <v>98.9</v>
+        <v>179.89</v>
       </c>
       <c r="H11">
-        <v>1.7798</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1613000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12">
-        <v>1.7430000000000001</v>
+        <v>2.84</v>
       </c>
       <c r="C12">
-        <v>85.21</v>
+        <v>164.23</v>
       </c>
       <c r="D12">
-        <v>1.5248999999999999</v>
+        <v>2.1371000000000002</v>
       </c>
       <c r="E12">
-        <v>7.8E-2</v>
+        <v>-2.12E-2</v>
       </c>
       <c r="F12">
-        <v>8.6E-3</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="G12">
-        <v>98.21</v>
+        <v>179.23</v>
       </c>
       <c r="H12">
-        <v>1.7730999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1638000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13">
-        <v>1.762</v>
+        <v>2.7509999999999999</v>
       </c>
       <c r="C13">
-        <v>84.41</v>
+        <v>164.17</v>
       </c>
       <c r="D13">
-        <v>1.5286</v>
+        <v>2.1318000000000001</v>
       </c>
       <c r="E13">
-        <v>7.3700000000000002E-2</v>
+        <v>-1.9199999999999998E-2</v>
       </c>
       <c r="F13">
-        <v>9.1000000000000004E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="G13">
-        <v>97.41</v>
+        <v>179.17</v>
       </c>
       <c r="H13">
-        <v>1.7694000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1619999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14">
-        <v>2.1240000000000001</v>
+        <v>2.7149999999999999</v>
       </c>
       <c r="C14">
-        <v>84.29</v>
+        <v>164.75</v>
       </c>
       <c r="D14">
-        <v>1.532</v>
+        <v>2.1074999999999999</v>
       </c>
       <c r="E14">
-        <v>7.6799999999999993E-2</v>
+        <v>-8.2000000000000007E-3</v>
       </c>
       <c r="F14">
-        <v>8.5000000000000006E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="G14">
-        <v>97.29</v>
+        <v>179.75</v>
       </c>
       <c r="H14">
-        <v>1.7766999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1570999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15">
-        <v>1.89</v>
+        <v>2.5419999999999998</v>
       </c>
       <c r="C15">
-        <v>84.81</v>
+        <v>165.74</v>
       </c>
       <c r="D15">
-        <v>1.5357000000000001</v>
+        <v>2.1105</v>
       </c>
       <c r="E15">
-        <v>7.9299999999999995E-2</v>
+        <v>-8.0999999999999996E-3</v>
       </c>
       <c r="F15">
-        <v>7.6E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G15">
-        <v>97.81</v>
+        <v>180.74</v>
       </c>
       <c r="H15">
-        <v>1.7813000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1589999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16">
-        <v>1.7290000000000001</v>
+        <v>2.214</v>
       </c>
       <c r="C16">
-        <v>84.56</v>
+        <v>167.55</v>
       </c>
       <c r="D16">
-        <v>1.5928</v>
+        <v>2.0714000000000001</v>
       </c>
       <c r="E16">
-        <v>5.5500000000000001E-2</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="F16">
-        <v>8.8999999999999999E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="G16">
-        <v>97.56</v>
+        <v>182.55</v>
       </c>
       <c r="H16">
-        <v>1.7866</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1493000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17">
-        <v>1.869</v>
+        <v>2.3159999999999998</v>
       </c>
       <c r="C17">
-        <v>84.39</v>
+        <v>165.95</v>
       </c>
       <c r="D17">
-        <v>1.5633999999999999</v>
+        <v>2.0708000000000002</v>
       </c>
       <c r="E17">
-        <v>7.5600000000000001E-2</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="F17">
-        <v>7.1000000000000004E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="G17">
-        <v>97.39</v>
+        <v>180.95</v>
       </c>
       <c r="H17">
-        <v>1.7965</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1486000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18">
-        <v>1.619</v>
+        <v>2.5760000000000001</v>
       </c>
       <c r="C18">
-        <v>83.83</v>
+        <v>163.25</v>
       </c>
       <c r="D18">
-        <v>1.5407</v>
+        <v>2.1017999999999999</v>
       </c>
       <c r="E18">
-        <v>6.7400000000000002E-2</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="F18">
-        <v>9.2999999999999992E-3</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="G18">
-        <v>96.83</v>
+        <v>178.25</v>
       </c>
       <c r="H18">
-        <v>1.7673000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1522999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19">
-        <v>1.8240000000000001</v>
+        <v>2.6819999999999999</v>
       </c>
       <c r="C19">
-        <v>83.52</v>
+        <v>161.94999999999999</v>
       </c>
       <c r="D19">
-        <v>1.5436000000000001</v>
+        <v>2.1417000000000002</v>
       </c>
       <c r="E19">
-        <v>6.7400000000000002E-2</v>
+        <v>-2.6200000000000001E-2</v>
       </c>
       <c r="F19">
-        <v>9.4999999999999998E-3</v>
+        <v>1.34E-2</v>
       </c>
       <c r="G19">
-        <v>96.52</v>
+        <v>176.95</v>
       </c>
       <c r="H19">
-        <v>1.7713000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20">
-        <v>1.9350000000000001</v>
+        <v>2.6869999999999998</v>
       </c>
       <c r="C20">
-        <v>84.88</v>
+        <v>162.58000000000001</v>
       </c>
       <c r="D20">
-        <v>1.5344</v>
+        <v>2.1423000000000001</v>
       </c>
       <c r="E20">
-        <v>7.5399999999999995E-2</v>
+        <v>-2.6499999999999999E-2</v>
       </c>
       <c r="F20">
-        <v>8.5000000000000006E-3</v>
+        <v>1.34E-2</v>
       </c>
       <c r="G20">
-        <v>97.88</v>
+        <v>177.58</v>
       </c>
       <c r="H20">
-        <v>1.7757000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21">
-        <v>1.718</v>
+        <v>2.7210000000000001</v>
       </c>
       <c r="C21">
-        <v>86.98</v>
+        <v>163.56</v>
       </c>
       <c r="D21">
-        <v>1.5325</v>
+        <v>2.1173000000000002</v>
       </c>
       <c r="E21">
-        <v>7.6399999999999996E-2</v>
+        <v>-1.54E-2</v>
       </c>
       <c r="F21">
-        <v>8.3000000000000001E-3</v>
+        <v>1.21E-2</v>
       </c>
       <c r="G21">
-        <v>99.98</v>
+        <v>178.56</v>
       </c>
       <c r="H21">
-        <v>1.7750999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1541999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22">
-        <v>1.7030000000000001</v>
+        <v>2.782</v>
       </c>
       <c r="C22">
-        <v>87.47</v>
+        <v>164.84</v>
       </c>
       <c r="D22">
-        <v>1.5396000000000001</v>
+        <v>2.1196000000000002</v>
       </c>
       <c r="E22">
-        <v>8.4500000000000006E-2</v>
+        <v>-1.44E-2</v>
       </c>
       <c r="F22">
-        <v>6.4000000000000003E-3</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="G22">
-        <v>100.47</v>
+        <v>179.84</v>
       </c>
       <c r="H22">
-        <v>1.7907</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2.1576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23">
-        <v>1.9179999999999999</v>
+        <v>2.6419999999999999</v>
       </c>
       <c r="C23">
-        <v>85.77</v>
+        <v>166.04</v>
       </c>
       <c r="D23">
-        <v>1.5713999999999999</v>
+        <v>2.0743</v>
       </c>
       <c r="E23">
-        <v>7.4700000000000003E-2</v>
+        <v>6.3E-3</v>
       </c>
       <c r="F23">
-        <v>6.7999999999999996E-3</v>
+        <v>9.1999999999999998E-3</v>
       </c>
       <c r="G23">
-        <v>98.77</v>
+        <v>181.04</v>
       </c>
       <c r="H23">
-        <v>1.8005</v>
+        <v>2.1474000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>